<commit_message>
fix plot include timestamp by accident
</commit_message>
<xml_diff>
--- a/excel/pana_log.xlsx
+++ b/excel/pana_log.xlsx
@@ -11,6 +11,7 @@
     <sheet name="2023-12-15 10_26_58" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2023-12-15 10_50_14" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2023-12-15 16_39_07" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2023-12-18 09_45_00" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -480,7 +481,6 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -551,6 +551,147 @@
           <val>
             <numRef>
               <f>'2023-12-15 16_39_07'!$C$2:$C$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Test number</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>PM 2.5 (µg/m³)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Panasonic SN-GCJA5 Test Sample 0</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'2023-12-18 09_45_00'!C1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'2023-12-18 09_45_00'!$C$2:$C$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'2023-12-18 09_45_00'!D1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'2023-12-18 09_45_00'!$D$2:$D$11</f>
             </numRef>
           </val>
         </ser>
@@ -701,6 +842,33 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>12</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1951,4 +2119,201 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5.421000003814697</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_49</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5.598999977111816</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_50</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5.959000110626221</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_51</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6.171999931335449</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_52</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6.349999904632568</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_54</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5.633999824523926</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_55</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5.781000137329102</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_56</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5.390999794006348</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_57</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5.034999847412109</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_44_58</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5.034999847412109</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2023-12-18 09_45_00</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>